<commit_message>
Rédaction + tts df1 et df2
</commit_message>
<xml_diff>
--- a/assets/df_a_constituer.xlsx
+++ b/assets/df_a_constituer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pascal.irz\Documents\projets\ASPE\package\aspe_demo\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D6C85A-77A7-455B-93B0-8F7207D4E074}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44183801-026B-4122-8A5F-C151B1350F08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{12AA6E70-DA7C-494B-8483-5032EE91F0A8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{12AA6E70-DA7C-494B-8483-5032EE91F0A8}"/>
   </bookViews>
   <sheets>
     <sheet name="1_1sp_1ope" sheetId="1" r:id="rId1"/>
@@ -837,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B59647-B2CA-4A34-A46E-1C2672E0AE43}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,13 +928,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>83</v>
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -959,135 +959,135 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" t="s">
-        <v>139</v>
-      </c>
-    </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" t="s">
-        <v>141</v>
+        <v>52</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>142</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>16</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>65</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C25" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1296,7 +1296,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A4" sqref="A4:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1534,7 +1534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA13DBD-20DC-4C65-8406-6526B6A6FCB1}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
20 : avancé sur stats tailles et param envt
</commit_message>
<xml_diff>
--- a/assets/df_a_constituer.xlsx
+++ b/assets/df_a_constituer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pascal.irz\Documents\projets\ASPE\package\aspe_demo\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44183801-026B-4122-8A5F-C151B1350F08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E88D378-5C49-4801-A04B-6B18EAB7C586}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{12AA6E70-DA7C-494B-8483-5032EE91F0A8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{12AA6E70-DA7C-494B-8483-5032EE91F0A8}"/>
   </bookViews>
   <sheets>
     <sheet name="1_1sp_1ope" sheetId="1" r:id="rId1"/>
@@ -142,9 +142,6 @@
     <t>b_moy</t>
   </si>
   <si>
-    <t>richesse_moy</t>
-  </si>
-  <si>
     <t>effectif_moy</t>
   </si>
   <si>
@@ -467,6 +464,9 @@
   </si>
   <si>
     <t>Synthèse peuplement par opération</t>
+  </si>
+  <si>
+    <t>richesse_moy  (diversité alpha)</t>
   </si>
 </sst>
 </file>
@@ -837,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B59647-B2CA-4A34-A46E-1C2672E0AE43}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,238 +857,238 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>137</v>
+        <v>70</v>
+      </c>
+      <c r="C7" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>83</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" t="s">
-        <v>84</v>
+        <v>50</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>82</v>
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" t="s">
-        <v>140</v>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" t="s">
-        <v>139</v>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>83</v>
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" t="s">
-        <v>85</v>
+        <v>51</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
         <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>142</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>16</v>
       </c>
-      <c r="B25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" t="s">
-        <v>142</v>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1099,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F59FDB6F-FCA9-46BB-82A5-47463DFC3C14}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,18 +1118,18 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1137,10 +1137,10 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1148,10 +1148,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1159,10 +1159,10 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1170,120 +1170,120 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>121</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>121</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" t="s">
-        <v>143</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1296,7 +1296,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C21"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,18 +1313,18 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1332,10 +1332,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1343,10 +1343,10 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1354,10 +1354,10 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1365,10 +1365,10 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1376,10 +1376,10 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1387,10 +1387,10 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1398,10 +1398,10 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1409,10 +1409,10 @@
         <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1420,10 +1420,10 @@
         <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1431,21 +1431,21 @@
         <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" t="s">
         <v>125</v>
       </c>
-      <c r="B14" t="s">
-        <v>126</v>
-      </c>
       <c r="C14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1453,10 +1453,10 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1464,10 +1464,10 @@
         <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1475,10 +1475,10 @@
         <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1486,10 +1486,10 @@
         <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1497,10 +1497,10 @@
         <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1508,10 +1508,10 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1519,10 +1519,10 @@
         <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1534,8 +1534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA13DBD-20DC-4C65-8406-6526B6A6FCB1}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,18 +1555,18 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1574,164 +1574,164 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" t="s">
         <v>106</v>
       </c>
-      <c r="B8" t="s">
-        <v>107</v>
-      </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>